<commit_message>
TIVA based Daughter Manual Board First Draft
</commit_message>
<xml_diff>
--- a/Sensor List.xlsx
+++ b/Sensor List.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="90">
   <si>
     <t>IR Proximity Sensors</t>
   </si>
@@ -241,6 +241,51 @@
   </si>
   <si>
     <t>Sharp IR range sensor 2</t>
+  </si>
+  <si>
+    <t>Plug and Play</t>
+  </si>
+  <si>
+    <t>uC based</t>
+  </si>
+  <si>
+    <t>Pin</t>
+  </si>
+  <si>
+    <t>RX</t>
+  </si>
+  <si>
+    <t>TX</t>
+  </si>
+  <si>
+    <t>PB0(UART1)</t>
+  </si>
+  <si>
+    <t>PB1(UART1)</t>
+  </si>
+  <si>
+    <t>PC6(UART3)</t>
+  </si>
+  <si>
+    <t>PC7(UART3)</t>
+  </si>
+  <si>
+    <t>SCL</t>
+  </si>
+  <si>
+    <t>SDA</t>
+  </si>
+  <si>
+    <t>PB3(I2C0)</t>
+  </si>
+  <si>
+    <t>PB2(I2C0)</t>
+  </si>
+  <si>
+    <t>PA6(I2C1)</t>
+  </si>
+  <si>
+    <t>PA7(I2C1)</t>
   </si>
 </sst>
 </file>
@@ -591,10 +636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J49"/>
+  <dimension ref="A1:N49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,9 +650,11 @@
     <col min="6" max="6" width="15.5703125" customWidth="1"/>
     <col min="8" max="8" width="26.5703125" customWidth="1"/>
     <col min="10" max="10" width="28" customWidth="1"/>
+    <col min="13" max="13" width="14" customWidth="1"/>
+    <col min="14" max="14" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -624,7 +671,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -650,7 +697,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -675,8 +722,17 @@
       <c r="J3" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -701,8 +757,17 @@
       <c r="J4" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L4" t="s">
+        <v>78</v>
+      </c>
+      <c r="M4" t="s">
+        <v>80</v>
+      </c>
+      <c r="N4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -727,8 +792,17 @@
       <c r="J5" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L5" t="s">
+        <v>79</v>
+      </c>
+      <c r="M5" t="s">
+        <v>81</v>
+      </c>
+      <c r="N5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -754,7 +828,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -780,7 +854,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -805,8 +879,17 @@
       <c r="J8" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L8" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="N8" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -831,8 +914,17 @@
       <c r="J9" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L9" t="s">
+        <v>84</v>
+      </c>
+      <c r="M9" t="s">
+        <v>88</v>
+      </c>
+      <c r="N9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F10" s="2">
         <v>7</v>
       </c>
@@ -848,8 +940,17 @@
       <c r="J10" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L10" t="s">
+        <v>85</v>
+      </c>
+      <c r="M10" t="s">
+        <v>89</v>
+      </c>
+      <c r="N10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F11" s="2">
         <v>8</v>
       </c>
@@ -866,7 +967,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="F12" s="2">
         <v>9</v>
       </c>
@@ -883,7 +984,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>15</v>
       </c>
@@ -909,7 +1010,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
@@ -935,7 +1036,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
@@ -946,7 +1047,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>3</v>
       </c>

</xml_diff>